<commit_message>
Running Home & Login
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestingData.xlsx
+++ b/src/test/resources/TestData/TestingData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onlin\eclipse-workspace\DsAlgo_Galaxy\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB735728-0C73-41B1-8590-B0F7701F293C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C05992-EB62-4C7A-A6FD-F766B735BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -467,16 +469,16 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -498,7 +500,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -508,7 +510,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -520,7 +522,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -532,7 +534,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -544,7 +546,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -556,7 +558,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -568,7 +570,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -583,4 +585,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB5C662-2F1E-4CFF-8416-7834CF626327}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4021EB5-FFC0-442B-8BA4-F9B02CB7FCEA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Register and signin Link
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestingData.xlsx
+++ b/src/test/resources/TestData/TestingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onlin\eclipse-workspace\DsAlgo_Galaxy\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C05992-EB62-4C7A-A6FD-F766B735BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E777E71-F865-4670-9C76-E2AED6A42446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -50,61 +50,10 @@
     <t>errorMsg</t>
   </si>
   <si>
-    <t>Testing1</t>
-  </si>
-  <si>
     <t>Testing12</t>
   </si>
   <si>
     <t>Test123</t>
-  </si>
-  <si>
-    <t>fcbhgug5mkji</t>
-  </si>
-  <si>
-    <t>Testing1234</t>
-  </si>
-  <si>
-    <t>Testing12345</t>
-  </si>
-  <si>
-    <t>test23</t>
-  </si>
-  <si>
-    <t>Testing2968</t>
-  </si>
-  <si>
-    <t>test9087</t>
-  </si>
-  <si>
-    <t>Testing@2025!</t>
-  </si>
-  <si>
-    <t>Welcome@25!</t>
-  </si>
-  <si>
-    <t>admin1</t>
-  </si>
-  <si>
-    <t>Welcome1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Testing123</t>
-  </si>
-  <si>
-    <t>welcomehere</t>
-  </si>
-  <si>
-    <t>Welcome</t>
-  </si>
-  <si>
-    <t>well00125</t>
-  </si>
-  <si>
-    <t>Querty#11</t>
-  </si>
-  <si>
-    <t>Galaxy1</t>
   </si>
 </sst>
 </file>
@@ -469,16 +418,16 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,94 +441,56 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>191673</v>
-      </c>
-      <c r="C5" s="2">
-        <v>25963</v>
-      </c>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
   </sheetData>
@@ -593,7 +504,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -605,7 +516,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sign in positive scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestingData.xlsx
+++ b/src/test/resources/TestData/TestingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onlin\eclipse-workspace\DsAlgo_Galaxy\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E777E71-F865-4670-9C76-E2AED6A42446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F39EF4-2CE8-4409-A25A-DF2A02EA7F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Test123</t>
+  </si>
+  <si>
+    <t>We_team3</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy</t>
   </si>
 </sst>
 </file>
@@ -418,7 +424,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,8 +448,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>

</xml_diff>

<commit_message>
code ready to push
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestingData.xlsx
+++ b/src/test/resources/TestData/TestingData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onlin\eclipse-workspace\DsAlgo_Galaxy\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0DD976-6EA8-489B-A0D7-0A6B78EE85F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C6F0BD-1038-4968-A008-3AEB1EA4C3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="tryEditorCode" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -44,29 +44,71 @@
     <t>password</t>
   </si>
   <si>
+    <t>This is a test message !</t>
+  </si>
+  <si>
+    <t>print('Python is fun!');</t>
+  </si>
+  <si>
+    <t>editorCode</t>
+  </si>
+  <si>
+    <t>We_team3</t>
+  </si>
+  <si>
     <t>password confirmation</t>
   </si>
   <si>
-    <t>errorMsg</t>
-  </si>
-  <si>
-    <t>Testing12</t>
-  </si>
-  <si>
-    <t>Test123</t>
-  </si>
-  <si>
-    <t>We_team3</t>
+    <t>NumpyNinja</t>
+  </si>
+  <si>
+    <t>NinjaGalaxy</t>
+  </si>
+  <si>
+    <t>Querty1</t>
+  </si>
+  <si>
+    <t>Ninja Galaxy</t>
   </si>
   <si>
     <t>Ninja_Galaxy</t>
+  </si>
+  <si>
+    <t>testingdemo</t>
+  </si>
+  <si>
+    <t>testingdemo123</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy123</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy14</t>
+  </si>
+  <si>
+    <t>wert</t>
+  </si>
+  <si>
+    <t>csfa</t>
+  </si>
+  <si>
+    <t>rtaa</t>
+  </si>
+  <si>
+    <t>rwerqw</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +121,44 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,17 +178,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,87 +514,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CD3947-FABD-4E43-9D5C-96775582D864}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -510,24 +601,146 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB5C662-2F1E-4CFF-8416-7834CF626327}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4021EB5-FFC0-442B-8BA4-F9B02CB7FCEA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8">
+        <v>259603</v>
+      </c>
+      <c r="C7" s="8">
+        <v>259603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pushing complete local project to Pramodini branch 4th May
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestingData.xlsx
+++ b/src/test/resources/TestData/TestingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshdeshmukh/eclipse-workspace/NinjaGalaxy-Jaanvi-branch/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8843765-0A87-8542-B028-498139767CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF83349-EDB1-F747-8875-A2CCBD2396FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
+    <workbookView xWindow="4140" yWindow="500" windowWidth="31700" windowHeight="19920" activeTab="4" xr2:uid="{C2348D72-976D-4F37-A81F-BEBD0C413FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -46,49 +46,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Password confirmation</t>
-  </si>
-  <si>
     <t>We_team3</t>
-  </si>
-  <si>
-    <t>testuser</t>
-  </si>
-  <si>
-    <t>tu123</t>
-  </si>
-  <si>
-    <t>tu321</t>
-  </si>
-  <si>
-    <t>""</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sername</t>
-    </r>
-  </si>
-  <si>
-    <t>pCode</t>
   </si>
   <si>
     <t>print("hello");</t>
@@ -105,58 +63,190 @@
 search([12, 23, 45, 67, 6, 90], 12)</t>
   </si>
   <si>
+    <t>Ninja_galaxy</t>
+  </si>
+  <si>
+    <t>gjdgqhgdqdq</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
     <t>def search(input_list, num):
-if(num in input_list):
-print("Element Found")
-\xc
-\xc
-else:
-print("Not Found")
-\xc
-\xc
-\xc
-\xc
-search([12, 23, 45, 67, 6, 90] , 12)</t>
-  </si>
-  <si>
-    <t>pcode</t>
-  </si>
-  <si>
-    <t>def findMaxConsecutiveOnes(nums) :
-count = 0
-result = 0
-for i in range(0, len(nums)):
-if (nums[i] == 0):
-count = 0
-\xc
-\xc
-else:
-count+= 1
-\xc
-\xc
-result = max(result, count)
-\xc
-\xc
-print(result)
-\xc
-\xc
-findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Some Tests failed. Please review code</t>
-  </si>
-  <si>
-    <t>Ninja_galaxy</t>
-  </si>
-  <si>
-    <t>Ninja_Galaxy13</t>
+    if num in input_list:
+        print("Element Found")
+search([12, 23, 45, 67, 6, 90], 50)</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    count = 0  # To keep track of the current consecutive 1s
+    max_count = 0  # To store the maximum consecutive 1s
+    for num in nums:
+        if num == 1:
+            count += 1  # Increment count if the current element is 1
+        else:
+            max_count = max(max_count, count)  # Update max_count if necessary
+            count = 0  # Reset the count when a 0 is encountered
+    max_count = max(max_count, count)  # Final update in case array ends with 1s
+    return max_count
+# Example Test Cases
+print(findMaxConsecutiveOnes([1, 1, 0, 1, 1, 1]))  # Output: 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def sortedSquares(nums):
+    n = len(nums)
+    result = [0] * n
+    left, right = 0, n - 1
+    pos = n - 1
+    while left &lt;= right:
+        left_sq = nums[left] ** 2
+        right_sq = nums[right] ** 2
+        if left_sq &gt; right_sq:
+            result[pos] = left_sq
+            left += 1
+        else:
+            result[pos] = right_sq
+            right -= 1
+        pos -= 1
+    return result 
+print(sortedSquares([-4,-1,0,3,10]))   # Output: [0, 1, 9, 16, 100]
+print(sortedSquares([-7,-3,2,3,11]))   # Output: [4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def findNumbers(nums):
+    count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            count += 1
+    return count
+print(findNumbers([12, 345, 2, 6, 7896]))       
+print(findNumbers([555, 901, 482, 1771]))  </t>
+  </si>
+  <si>
+    <t>password confirmation</t>
+  </si>
+  <si>
+    <t>errorMsg</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Feature File</t>
+  </si>
+  <si>
+    <t>scenario number</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>Register when All fields empty</t>
+  </si>
+  <si>
+    <t>Register when only username filed is entered</t>
+  </si>
+  <si>
+    <t>Register when confirmation password field is empty</t>
+  </si>
+  <si>
+    <t>fcbhgug5mkji</t>
+  </si>
+  <si>
+    <t> fcbhgug5mkji</t>
+  </si>
+  <si>
+    <t>Username entered with spaces</t>
+  </si>
+  <si>
+    <t>only numeric password</t>
+  </si>
+  <si>
+    <t>test23</t>
+  </si>
+  <si>
+    <t>less than 8 char pswd</t>
+  </si>
+  <si>
+    <t>test34567</t>
+  </si>
+  <si>
+    <t>test9087</t>
+  </si>
+  <si>
+    <t>Different pwds in both password fields</t>
+  </si>
+  <si>
+    <t>Welcome@25!</t>
+  </si>
+  <si>
+    <t>Valid info is filled in all fields</t>
+  </si>
+  <si>
+    <t>admin1</t>
+  </si>
+  <si>
+    <t>click SignIn  button from registartion</t>
+  </si>
+  <si>
+    <t>admin2</t>
+  </si>
+  <si>
+    <t>Welcome2</t>
+  </si>
+  <si>
+    <t>clickLogin button from registration page.</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy123</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy1234</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy12345</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy2968</t>
+  </si>
+  <si>
+    <t>Ninja_Galaxy@2025!</t>
+  </si>
+  <si>
+    <t>Welcome3</t>
+  </si>
+  <si>
+    <t>testuser</t>
+  </si>
+  <si>
+    <t>hghdgihd</t>
+  </si>
+  <si>
+    <t>dqdqd</t>
+  </si>
+  <si>
+    <t>Ninja_galaxy122</t>
+  </si>
+  <si>
+    <t>Ninja     Galaxy</t>
+  </si>
+  <si>
+    <t>editorCode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,27 +261,55 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -199,11 +317,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -218,8 +352,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,65 +687,234 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB5C662-2F1E-4CFF-8416-7834CF626327}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="185" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14" style="10" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="9">
+        <v>25963</v>
+      </c>
+      <c r="C7" s="9">
+        <v>25963</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="8">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -599,15 +922,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CD3947-FABD-4E43-9D5C-96775582D864}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,48 +946,64 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
@@ -672,6 +1012,30 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -683,9 +1047,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
+    <sheetView zoomScale="273" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -694,17 +1056,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -715,28 +1077,45 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1341CD10-02E0-0644-BFA9-113813FCDB69}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.6640625" customWidth="1"/>
+    <col min="1" max="1" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="112" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="4" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="4" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="4" customFormat="1" ht="256" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -749,30 +1128,27 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="47.1640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="54.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-    </row>
-    <row r="2" spans="1:2" ht="192" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="335" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="249" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="160" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>